<commit_message>
adding a simplex solution
</commit_message>
<xml_diff>
--- a/Simplex_Method_QMBE_3730.xlsx
+++ b/Simplex_Method_QMBE_3730.xlsx
@@ -8,13 +8,46 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodge\OneDrive\Desktop\QMBE 3750 Kennedy Odongo\QMBE-3750-Kennedy-Odongo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3EA81B39-8F01-4C58-8790-16F7C790E255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09DCD257-F75E-4EEC-B071-8A6626FAE292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5063B314-E7F7-4543-8D97-F80CAAB7BDB5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Answer Report 1" sheetId="2" r:id="rId1"/>
+    <sheet name="What if model with Excel Solver" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">'What if model with Excel Solver'!$B$14:$C$14</definedName>
+    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">'What if model with Excel Solver'!$B$19:$B$22</definedName>
+    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">'What if model with Excel Solver'!$B$16</definedName>
+    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">'What if model with Excel Solver'!$C$19:$C$22</definedName>
+    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,12 +68,222 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="63">
+  <si>
+    <t>Par, Inc.</t>
+  </si>
+  <si>
+    <t>Parameters</t>
+  </si>
+  <si>
+    <t>Operation</t>
+  </si>
+  <si>
+    <t>Cutting and Dyeing</t>
+  </si>
+  <si>
+    <t>Sewing</t>
+  </si>
+  <si>
+    <t>Finishing</t>
+  </si>
+  <si>
+    <t>Inspection and Packaging</t>
+  </si>
+  <si>
+    <t>Profit per pag</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>Deluxe</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Production Time in Hours</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Bags Produced</t>
+  </si>
+  <si>
+    <t>Total Profit</t>
+  </si>
+  <si>
+    <t>Hours Used</t>
+  </si>
+  <si>
+    <t>Hours Available</t>
+  </si>
+  <si>
+    <t>Decision Variables</t>
+  </si>
+  <si>
+    <t>Objective Function</t>
+  </si>
+  <si>
+    <t>Microsoft Excel 16.0 Answer Report</t>
+  </si>
+  <si>
+    <t>Worksheet: [Simplex_Method_QMBE_3730.xlsx]What if model with Excel Solver</t>
+  </si>
+  <si>
+    <t>Report Created: 4/16/2024 10:17:50 AM</t>
+  </si>
+  <si>
+    <t>Result: Solver found a solution.  All Constraints and optimality conditions are satisfied.</t>
+  </si>
+  <si>
+    <t>Solver Engine</t>
+  </si>
+  <si>
+    <t>Engine: Simplex LP</t>
+  </si>
+  <si>
+    <t>Solution Time: 0 Seconds.</t>
+  </si>
+  <si>
+    <t>Iterations: 2 Subproblems: 0</t>
+  </si>
+  <si>
+    <t>Solver Options</t>
+  </si>
+  <si>
+    <t>Max Time Unlimited,  Iterations Unlimited, Precision 0.000001, Use Automatic Scaling</t>
+  </si>
+  <si>
+    <t>Max Subproblems Unlimited, Max Integer Sols Unlimited, Integer Tolerance 1%, Assume NonNegative</t>
+  </si>
+  <si>
+    <t>Objective Cell (Max)</t>
+  </si>
+  <si>
+    <t>Cell</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Original Value</t>
+  </si>
+  <si>
+    <t>Final Value</t>
+  </si>
+  <si>
+    <t>Variable Cells</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>Constraints</t>
+  </si>
+  <si>
+    <t>Cell Value</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Slack</t>
+  </si>
+  <si>
+    <t>$B$16</t>
+  </si>
+  <si>
+    <t>Total Profit Standard</t>
+  </si>
+  <si>
+    <t>$B$14</t>
+  </si>
+  <si>
+    <t>Bags Produced Standard</t>
+  </si>
+  <si>
+    <t>Contin</t>
+  </si>
+  <si>
+    <t>$C$14</t>
+  </si>
+  <si>
+    <t>Bags Produced Deluxe</t>
+  </si>
+  <si>
+    <t>$B$19</t>
+  </si>
+  <si>
+    <t>Cutting and Dyeing Hours Used</t>
+  </si>
+  <si>
+    <t>$B$19&lt;=$C$19</t>
+  </si>
+  <si>
+    <t>Binding</t>
+  </si>
+  <si>
+    <t>$B$20</t>
+  </si>
+  <si>
+    <t>Sewing Hours Used</t>
+  </si>
+  <si>
+    <t>$B$20&lt;=$C$20</t>
+  </si>
+  <si>
+    <t>Not Binding</t>
+  </si>
+  <si>
+    <t>$B$21</t>
+  </si>
+  <si>
+    <t>Finishing Hours Used</t>
+  </si>
+  <si>
+    <t>$B$21&lt;=$C$21</t>
+  </si>
+  <si>
+    <t>$B$22</t>
+  </si>
+  <si>
+    <t>Inspection and Packaging Hours Used</t>
+  </si>
+  <si>
+    <t>$B$22&lt;=$C$22</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="18"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -54,7 +297,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -62,12 +305,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="23"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="23"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="23"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,13 +683,501 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F6A60E7-ECE7-4A4D-AC08-F2CF44EFE01C}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C7C1991-3880-42A5-AF33-960205A7E74F}">
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="5">
+        <v>7668</v>
+      </c>
+      <c r="E16" s="5">
+        <v>7668</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="6">
+        <v>540</v>
+      </c>
+      <c r="E21" s="6">
+        <v>540</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="5">
+        <v>252</v>
+      </c>
+      <c r="E22" s="5">
+        <v>252</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="6">
+        <v>630</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G27" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="6">
+        <v>480</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G28" s="4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" s="6">
+        <v>708</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G29" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" s="5">
+        <v>117</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G30" s="2">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F6A60E7-ECE7-4A4D-AC08-F2CF44EFE01C}">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="24.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <f>7/10</f>
+        <v>0.7</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <f>5/10</f>
+        <v>0.5</v>
+      </c>
+      <c r="C6">
+        <f>5/6</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D6">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <f>2/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D7">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <f>1/10</f>
+        <v>0.1</v>
+      </c>
+      <c r="C8">
+        <f>1/4</f>
+        <v>0.25</v>
+      </c>
+      <c r="D8">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>540</v>
+      </c>
+      <c r="C14">
+        <v>252</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <f>SUMPRODUCT(B9:C9,$B$14:$C$14)</f>
+        <v>7668</v>
+      </c>
+      <c r="D16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <f>SUMPRODUCT(B5:C5,$B$14:$C$14)</f>
+        <v>630</v>
+      </c>
+      <c r="C19">
+        <f>D5</f>
+        <v>630</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <f>SUMPRODUCT(B6:C6,$B$14:$C$14)</f>
+        <v>480</v>
+      </c>
+      <c r="C20">
+        <f>D6</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <f>SUMPRODUCT(B7:C7,$B$14:$C$14)</f>
+        <v>708</v>
+      </c>
+      <c r="C21">
+        <f>D7</f>
+        <v>708</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22">
+        <f t="shared" ref="B20:B22" si="0">SUMPRODUCT(B8:C8,$B$14:$C$14)</f>
+        <v>117</v>
+      </c>
+      <c r="C22">
+        <f>D8</f>
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>